<commit_message>
Tested a few account features and found a bug
</commit_message>
<xml_diff>
--- a/TestLogs.xlsx
+++ b/TestLogs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skewl\QA\QA-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F12F320-F5A8-41D2-9C80-B1C5E768AC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036E786B-F933-431F-A1F8-5D4F27DC8E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{358DB06D-F862-4BE4-B67A-C1F7B0930CE9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Test ID</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>These 2 tests confirm the only required field for a account is a username</t>
+  </si>
+  <si>
+    <t>CheckSelf</t>
+  </si>
+  <si>
+    <t>Information about example account is shown</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t>Error message says "Too few arguments"</t>
   </si>
 </sst>
 </file>
@@ -426,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D9E750-DFAD-4EFC-BBDD-DE53978B9E45}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,6 +501,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished my half and found a missing page
</commit_message>
<xml_diff>
--- a/TestLogs.xlsx
+++ b/TestLogs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skewl\QA\QA-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036E786B-F933-431F-A1F8-5D4F27DC8E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A07133-4036-42F7-B86D-DA7D711CAE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{358DB06D-F862-4BE4-B67A-C1F7B0930CE9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Test ID</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>Error message says "Too few arguments"</t>
+  </si>
+  <si>
+    <t>LogoLink</t>
+  </si>
+  <si>
+    <t>Opens a webpage</t>
+  </si>
+  <si>
+    <t>Error 404 no webpage is found</t>
+  </si>
+  <si>
+    <t>The logo is the  being clicked is the cool little batman</t>
   </si>
 </sst>
 </file>
@@ -438,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D9E750-DFAD-4EFC-BBDD-DE53978B9E45}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,6 +530,23 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>